<commit_message>
Awsome we are now somewhere
</commit_message>
<xml_diff>
--- a/PythonEnvProjects/OP/nifty_option_chain_data.xlsx
+++ b/PythonEnvProjects/OP/nifty_option_chain_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\pythonenv\PythonEnvProjects\OP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EE3D04-320B-4AE6-B16F-395490FD055F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4AB5AE-9DF2-44A2-B969-D311506BE0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{F4491AA1-0B0E-4EC4-990F-37AB9351E9D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{F4491AA1-0B0E-4EC4-990F-37AB9351E9D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_Nifty" sheetId="1" r:id="rId1"/>
@@ -4003,13 +4003,13 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
@@ -4119,7 +4119,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{83D816D1-979A-4D3A-A948-4D027004C7DC}" name="NIFTY_EXPIRY" displayName="NIFTY_EXPIRY" ref="U1:U19" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="U1:U19" xr:uid="{83D816D1-979A-4D3A-A948-4D027004C7DC}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{CA5D5028-247D-4740-A916-7F81DA4F0F52}" uniqueName="1" name="expiryDate" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{CA5D5028-247D-4740-A916-7F81DA4F0F52}" uniqueName="1" name="expiryDate" queryTableFieldId="1" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4129,7 +4129,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{230394A0-34FF-48B1-A80E-75D34417F28E}" name="NIFTY_P" displayName="NIFTY_P" ref="A1:B2" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B2" xr:uid="{230394A0-34FF-48B1-A80E-75D34417F28E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{95FBF4C3-1423-4A78-A022-569A55FC8FE4}" uniqueName="1" name="timestamp" queryTableFieldId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{95FBF4C3-1423-4A78-A022-569A55FC8FE4}" uniqueName="1" name="timestamp" queryTableFieldId="1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{31C1858D-5F2F-40B9-8E64-4BBDE0DBC646}" uniqueName="2" name="SYMBOL_PRICE" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4140,7 +4140,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9A0976F7-F6FD-4715-8DEF-08AF76239003}" name="Table4" displayName="Table4" ref="F1:G2" totalsRowShown="0">
   <autoFilter ref="F1:G2" xr:uid="{9A0976F7-F6FD-4715-8DEF-08AF76239003}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3462AD64-A098-487B-86AE-2EC7DA03ADFC}" name="ExpiryDate" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3462AD64-A098-487B-86AE-2EC7DA03ADFC}" name="ExpiryDate" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{213A479C-80DB-4DC1-93C2-E74CAD6E7A00}" name="No. of Strikes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -83668,7 +83668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805672AC-3083-40D5-93D9-2F5344E1C859}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -83819,11 +83819,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D153D668-3983-4B95-8AB5-77F797CAD002}">
   <dimension ref="D10:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="10" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D10" s="3" t="s">

</xml_diff>